<commit_message>
Added comments for review
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Product.xlsx
+++ b/tests/artifact/script/Product.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="858">
   <si>
     <t>target</t>
   </si>
@@ -2644,6 +2644,9 @@
     <t>Get the product details</t>
   </si>
   <si>
+    <t>What is the negative scenario here. Reading the activity name I am not able to understand?</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -2672,6 +2675,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>activity name missing</t>
   </si>
   <si>
     <t>10</t>
@@ -2809,7 +2815,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2877,6 +2883,27 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
@@ -3398,135 +3425,135 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3710,10 +3737,16 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3746,7 +3779,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4114,7 +4147,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6790,11 +6823,11 @@
   <sheetPr/>
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -6845,7 +6878,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -6955,7 +6988,7 @@
       <c r="N5" s="25"/>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" s="4" customFormat="1" ht="15.6" spans="3:15">
+    <row r="6" s="4" customFormat="1" ht="15.5" spans="3:15">
       <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
@@ -7153,7 +7186,7 @@
       <c r="N13" s="25"/>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" customFormat="1" ht="374.4" spans="1:15">
+    <row r="14" customFormat="1" ht="377" spans="1:15">
       <c r="A14" s="21"/>
       <c r="B14" s="7"/>
       <c r="C14" s="27" t="s">
@@ -7288,7 +7321,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>780</v>
@@ -7305,7 +7338,7 @@
     </row>
     <row r="20" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="27" t="s">
@@ -7330,7 +7363,7 @@
       <c r="N20" s="25"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" customFormat="1" ht="43.2" spans="1:15">
+    <row r="21" customFormat="1" ht="43.5" spans="1:15">
       <c r="A21" s="21"/>
       <c r="B21" s="7"/>
       <c r="C21" s="27" t="s">
@@ -7440,7 +7473,7 @@
         <v>49</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F25" s="29" t="s">
         <v>780</v>
@@ -7536,7 +7569,7 @@
     </row>
     <row r="29" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="21" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="27" t="s">
@@ -7549,7 +7582,7 @@
         <v>770</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -7574,7 +7607,7 @@
         <v>803</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="G30" s="28"/>
       <c r="H30" s="29"/>
@@ -7671,7 +7704,7 @@
         <v>49</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>780</v>
@@ -10642,11 +10675,11 @@
   <sheetPr/>
   <dimension ref="A1:XFD197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38" style="6" customWidth="1"/>
     <col min="2" max="2" width="44.125" style="7" customWidth="1"/>
@@ -10696,7 +10729,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>733</v>
       </c>
@@ -10777,7 +10810,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="5" s="53" customFormat="1" ht="32" customHeight="1" spans="1:16384">
+    <row r="5" s="56" customFormat="1" ht="32" customHeight="1" spans="1:16384">
       <c r="A5" s="21" t="s">
         <v>747</v>
       </c>
@@ -27225,7 +27258,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:15">
+    <row r="8" s="1" customFormat="1" ht="29" spans="1:15">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="27" t="s">
@@ -27300,7 +27333,7 @@
       <c r="N10" s="25"/>
       <c r="O10" s="24"/>
     </row>
-    <row r="11" s="4" customFormat="1" ht="15.6" spans="1:15">
+    <row r="11" s="4" customFormat="1" ht="15.5" spans="1:15">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="H11" s="29"/>
@@ -27312,7 +27345,7 @@
       <c r="N11" s="25"/>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" s="4" customFormat="1" ht="15.6" spans="1:15">
+    <row r="12" s="4" customFormat="1" ht="15.5" spans="1:15">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="H12" s="29"/>
@@ -27324,7 +27357,7 @@
       <c r="N12" s="25"/>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" customFormat="1" ht="15.6" spans="1:15">
+    <row r="13" customFormat="1" ht="15.5" spans="1:15">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="H13" s="29"/>
@@ -27337,8 +27370,8 @@
       <c r="O13" s="24"/>
     </row>
     <row r="14" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A14" s="54"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="58"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
       <c r="J14" s="46"/>
@@ -27349,13 +27382,13 @@
       <c r="O14" s="47"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A15" s="54"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="57"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
       <c r="J15" s="46"/>
@@ -27366,9 +27399,9 @@
       <c r="O15" s="47"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="59"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -27383,12 +27416,12 @@
       <c r="O16" s="47"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A17" s="54"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="62"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
@@ -27520,7 +27553,7 @@
     </row>
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="21"/>
-      <c r="B25" s="63"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="35"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -30517,11 +30550,11 @@
   <sheetPr/>
   <dimension ref="A1:O191"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A46" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -30572,7 +30605,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -31213,7 +31246,7 @@
       <c r="N26" s="25"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="27" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A27" s="21" t="s">
         <v>790</v>
       </c>
@@ -31417,7 +31450,7 @@
       <c r="N34" s="25"/>
       <c r="O34" s="24"/>
     </row>
-    <row r="35" customFormat="1" ht="374.4" spans="1:15">
+    <row r="35" customFormat="1" ht="377" spans="1:15">
       <c r="A35" s="21"/>
       <c r="B35" s="7"/>
       <c r="C35" s="27" t="s">
@@ -31542,7 +31575,7 @@
       <c r="N39" s="48"/>
       <c r="O39" s="47"/>
     </row>
-    <row r="40" customFormat="1" ht="115.2" spans="1:15">
+    <row r="40" customFormat="1" ht="116" spans="1:15">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="27" t="s">
@@ -34571,7 +34604,7 @@
       <selection activeCell="A5" sqref="A5:H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -34622,7 +34655,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -34809,7 +34842,7 @@
       <c r="N8" s="25"/>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="9" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A9" s="21" t="s">
         <v>810</v>
       </c>
@@ -35013,7 +35046,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" customFormat="1" ht="374.4" spans="1:15">
+    <row r="17" customFormat="1" ht="377" spans="1:15">
       <c r="A17" s="21"/>
       <c r="B17" s="7"/>
       <c r="C17" s="27" t="s">
@@ -35113,7 +35146,7 @@
       <c r="N20" s="48"/>
       <c r="O20" s="47"/>
     </row>
-    <row r="21" customFormat="1" ht="115.2" spans="1:15">
+    <row r="21" customFormat="1" ht="116" spans="1:15">
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
       <c r="C21" s="27" t="s">
@@ -35188,7 +35221,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="24" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A24" s="21"/>
       <c r="B24" s="22" t="s">
         <v>812</v>
@@ -35342,7 +35375,7 @@
       <c r="N29" s="25"/>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" customFormat="1" ht="259.2" spans="1:15">
+    <row r="30" customFormat="1" ht="261" spans="1:15">
       <c r="A30" s="21"/>
       <c r="B30" s="7"/>
       <c r="C30" s="27" t="s">
@@ -35442,7 +35475,7 @@
       <c r="N33" s="48"/>
       <c r="O33" s="47"/>
     </row>
-    <row r="34" customFormat="1" ht="115.2" spans="1:15">
+    <row r="34" customFormat="1" ht="116" spans="1:15">
       <c r="A34" s="21"/>
       <c r="B34" s="22"/>
       <c r="C34" s="27" t="s">
@@ -38724,7 +38757,7 @@
       <selection activeCell="A59" sqref="A59:G66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -38775,7 +38808,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -38962,7 +38995,7 @@
       <c r="N8" s="25"/>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="9" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A9" s="21" t="s">
         <v>810</v>
       </c>
@@ -39166,7 +39199,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" customFormat="1" ht="374.4" spans="1:15">
+    <row r="17" customFormat="1" ht="377" spans="1:15">
       <c r="A17" s="21"/>
       <c r="B17" s="7"/>
       <c r="C17" s="27" t="s">
@@ -39291,7 +39324,7 @@
       <c r="N21" s="48"/>
       <c r="O21" s="47"/>
     </row>
-    <row r="22" customFormat="1" ht="115.2" spans="1:15">
+    <row r="22" customFormat="1" ht="116" spans="1:15">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="27" t="s">
@@ -39422,7 +39455,7 @@
       <c r="N26" s="25"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" customFormat="1" ht="374.4" spans="1:15">
+    <row r="27" customFormat="1" ht="377" spans="1:15">
       <c r="A27" s="21"/>
       <c r="B27" s="7"/>
       <c r="C27" s="27" t="s">
@@ -39522,7 +39555,7 @@
       <c r="N30" s="48"/>
       <c r="O30" s="47"/>
     </row>
-    <row r="31" customFormat="1" ht="115.2" spans="1:15">
+    <row r="31" customFormat="1" ht="116" spans="1:15">
       <c r="A31" s="21"/>
       <c r="B31" s="22"/>
       <c r="C31" s="27" t="s">
@@ -39826,7 +39859,7 @@
       <c r="N42" s="25"/>
       <c r="O42" s="24"/>
     </row>
-    <row r="43" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="43" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A43" s="21" t="s">
         <v>822</v>
       </c>
@@ -40030,7 +40063,7 @@
       <c r="N50" s="25"/>
       <c r="O50" s="24"/>
     </row>
-    <row r="51" customFormat="1" ht="259.2" spans="1:15">
+    <row r="51" customFormat="1" ht="261" spans="1:15">
       <c r="A51" s="21"/>
       <c r="B51" s="7"/>
       <c r="C51" s="27" t="s">
@@ -40155,7 +40188,7 @@
       <c r="N55" s="48"/>
       <c r="O55" s="47"/>
     </row>
-    <row r="56" customFormat="1" ht="115.2" spans="1:15">
+    <row r="56" customFormat="1" ht="116" spans="1:15">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="27" t="s">
@@ -40284,7 +40317,7 @@
       <c r="N60" s="25"/>
       <c r="O60" s="24"/>
     </row>
-    <row r="61" customFormat="1" ht="259.2" spans="1:15">
+    <row r="61" customFormat="1" ht="261" spans="1:15">
       <c r="A61" s="21"/>
       <c r="B61" s="7"/>
       <c r="C61" s="27" t="s">
@@ -40384,7 +40417,7 @@
       <c r="N64" s="48"/>
       <c r="O64" s="47"/>
     </row>
-    <row r="65" customFormat="1" ht="115.2" spans="1:15">
+    <row r="65" customFormat="1" ht="116" spans="1:15">
       <c r="A65" s="21"/>
       <c r="B65" s="22"/>
       <c r="C65" s="27" t="s">
@@ -44106,7 +44139,7 @@
       <selection activeCell="B34" sqref="B34:E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -44157,7 +44190,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -44344,7 +44377,7 @@
       <c r="N8" s="25"/>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="9" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A9" s="21" t="s">
         <v>810</v>
       </c>
@@ -44548,7 +44581,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" customFormat="1" ht="374.4" spans="1:15">
+    <row r="17" customFormat="1" ht="377" spans="1:15">
       <c r="A17" s="21"/>
       <c r="B17" s="7"/>
       <c r="C17" s="27" t="s">
@@ -44673,7 +44706,7 @@
       <c r="N21" s="48"/>
       <c r="O21" s="47"/>
     </row>
-    <row r="22" customFormat="1" ht="115.2" spans="1:15">
+    <row r="22" customFormat="1" ht="116" spans="1:15">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="27" t="s">
@@ -44779,7 +44812,7 @@
       <c r="N25" s="25"/>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" customFormat="1" ht="43.2" spans="1:15">
+    <row r="26" customFormat="1" ht="43.5" spans="1:15">
       <c r="A26" s="21"/>
       <c r="B26" s="7"/>
       <c r="C26" s="27" t="s">
@@ -44879,7 +44912,7 @@
       <c r="N29" s="48"/>
       <c r="O29" s="47"/>
     </row>
-    <row r="30" customFormat="1" ht="115.2" spans="1:15">
+    <row r="30" customFormat="1" ht="116" spans="1:15">
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
       <c r="C30" s="27" t="s">
@@ -48103,11 +48136,11 @@
   <sheetPr/>
   <dimension ref="A1:O177"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -48158,7 +48191,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -48268,8 +48301,10 @@
       <c r="N5" s="25"/>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A6" s="21"/>
+    <row r="6" s="3" customFormat="1" ht="66" customHeight="1" spans="1:15">
+      <c r="A6" s="55" t="s">
+        <v>833</v>
+      </c>
       <c r="B6" s="22"/>
       <c r="C6" s="35" t="s">
         <v>5</v>
@@ -48376,7 +48411,7 @@
         <v>49</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>780</v>
@@ -48396,7 +48431,7 @@
         <v>783</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>5</v>
@@ -48420,8 +48455,10 @@
       <c r="N11" s="25"/>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A12" s="21"/>
+    <row r="12" s="3" customFormat="1" ht="46" customHeight="1" spans="1:15">
+      <c r="A12" s="55" t="s">
+        <v>833</v>
+      </c>
       <c r="B12" s="22"/>
       <c r="C12" s="35" t="s">
         <v>35</v>
@@ -48553,7 +48590,7 @@
         <v>49</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>780</v>
@@ -48568,7 +48605,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="18" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A18" s="21" t="s">
         <v>790</v>
       </c>
@@ -48597,8 +48634,10 @@
       <c r="N18" s="25"/>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" s="4" customFormat="1" ht="20" customHeight="1" spans="1:15">
-      <c r="A19" s="21"/>
+    <row r="19" s="4" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A19" s="55" t="s">
+        <v>833</v>
+      </c>
       <c r="B19" s="22"/>
       <c r="C19" s="27" t="s">
         <v>5</v>
@@ -48607,7 +48646,7 @@
         <v>465</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>794</v>
@@ -48907,7 +48946,7 @@
         <v>49</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>780</v>
@@ -48950,7 +48989,9 @@
       <c r="O32" s="47"/>
     </row>
     <row r="33" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A33" s="21"/>
+      <c r="A33" s="21" t="s">
+        <v>833</v>
+      </c>
       <c r="B33" s="22"/>
       <c r="C33" s="35" t="s">
         <v>35</v>
@@ -49032,7 +49073,7 @@
         <v>49</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>780</v>
@@ -49103,10 +49144,10 @@
     </row>
     <row r="39" s="1" customFormat="1" ht="32" customHeight="1" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C39" s="35" t="s">
         <v>5</v>
@@ -49118,7 +49159,7 @@
         <v>770</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
@@ -49213,7 +49254,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F43" s="29" t="s">
         <v>780</v>
@@ -49230,7 +49271,7 @@
     </row>
     <row r="44" s="1" customFormat="1" ht="36" customHeight="1" spans="1:15">
       <c r="A44" s="21" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="35" t="s">
@@ -49243,7 +49284,7 @@
         <v>770</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
@@ -49338,7 +49379,7 @@
         <v>49</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F48" s="29" t="s">
         <v>780</v>
@@ -51829,11 +51870,11 @@
   <sheetPr/>
   <dimension ref="A1:O198"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60:E60"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -51884,7 +51925,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -51967,7 +52008,7 @@
     </row>
     <row r="5" s="3" customFormat="1" ht="36" customHeight="1" spans="1:15">
       <c r="A5" s="21" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>791</v>
@@ -51994,7 +52035,7 @@
       <c r="N5" s="25"/>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" s="4" customFormat="1" ht="15.6" spans="3:15">
+    <row r="6" s="4" customFormat="1" ht="15.5" spans="3:15">
       <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
@@ -52027,7 +52068,7 @@
         <v>465</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>794</v>
@@ -52118,7 +52159,9 @@
       <c r="O10" s="24"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:15">
-      <c r="A11" s="21"/>
+      <c r="A11" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B11" s="22" t="s">
         <v>801</v>
       </c>
@@ -52302,7 +52345,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>780</v>
@@ -52342,8 +52385,10 @@
       <c r="N19" s="25"/>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" s="4" customFormat="1" ht="27.6" spans="1:15">
-      <c r="A20" s="21"/>
+    <row r="20" s="4" customFormat="1" ht="28" spans="1:15">
+      <c r="A20" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B20" s="22" t="s">
         <v>812</v>
       </c>
@@ -52379,7 +52424,7 @@
         <v>465</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>794</v>
@@ -52445,7 +52490,9 @@
       <c r="O23" s="24"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:15">
-      <c r="A24" s="21"/>
+      <c r="A24" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B24" s="22" t="s">
         <v>801</v>
       </c>
@@ -52496,7 +52543,7 @@
       <c r="N25" s="25"/>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" customFormat="1" ht="259.2" spans="1:15">
+    <row r="26" customFormat="1" ht="261" spans="1:15">
       <c r="A26" s="21"/>
       <c r="B26" s="7"/>
       <c r="C26" s="27" t="s">
@@ -52606,7 +52653,7 @@
         <v>49</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>780</v>
@@ -52739,7 +52786,7 @@
         <v>465</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>794</v>
@@ -52830,7 +52877,9 @@
       <c r="O38" s="24"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A39" s="21"/>
+      <c r="A39" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B39" s="22" t="s">
         <v>801</v>
       </c>
@@ -52917,7 +52966,7 @@
         <v>803</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="29"/>
@@ -53014,7 +53063,7 @@
         <v>49</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>780</v>
@@ -53055,7 +53104,9 @@
       <c r="O47" s="24"/>
     </row>
     <row r="48" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A48" s="21"/>
+      <c r="A48" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B48" s="22" t="s">
         <v>812</v>
       </c>
@@ -53091,7 +53142,7 @@
         <v>465</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F49" s="30" t="s">
         <v>794</v>
@@ -53157,7 +53208,9 @@
       <c r="O51" s="24"/>
     </row>
     <row r="52" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A52" s="21"/>
+      <c r="A52" s="55" t="s">
+        <v>844</v>
+      </c>
       <c r="B52" s="22" t="s">
         <v>801</v>
       </c>
@@ -53221,7 +53274,7 @@
         <v>803</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="29"/>
@@ -53318,7 +53371,7 @@
         <v>49</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F58" s="29" t="s">
         <v>780</v>
@@ -55969,11 +56022,11 @@
   <sheetPr/>
   <dimension ref="A1:O219"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:E79"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="7" customWidth="1"/>
@@ -56024,7 +56077,7 @@
       <c r="N1" s="16"/>
       <c r="O1" s="40"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>759</v>
       </c>
@@ -56134,7 +56187,10 @@
       <c r="N5" s="25"/>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" s="4" customFormat="1" ht="15.6" spans="3:15">
+    <row r="6" s="4" customFormat="1" ht="15.5" spans="1:15">
+      <c r="A6" s="53" t="s">
+        <v>833</v>
+      </c>
       <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
@@ -56167,7 +56223,7 @@
         <v>465</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>794</v>
@@ -56467,7 +56523,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>780</v>
@@ -56487,7 +56543,7 @@
         <v>817</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>5</v>
@@ -56511,7 +56567,10 @@
       <c r="N20" s="25"/>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+    <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A21" s="54" t="s">
+        <v>833</v>
+      </c>
       <c r="B21" s="33"/>
       <c r="C21" s="27" t="s">
         <v>5</v>
@@ -56645,7 +56704,7 @@
         <v>49</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>780</v>
@@ -56715,7 +56774,9 @@
       <c r="O28" s="47"/>
     </row>
     <row r="29" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A29" s="21"/>
+      <c r="A29" s="55" t="s">
+        <v>833</v>
+      </c>
       <c r="B29" s="22"/>
       <c r="C29" s="35" t="s">
         <v>5</v>
@@ -56822,7 +56883,7 @@
         <v>49</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>780</v>
@@ -56862,7 +56923,7 @@
       <c r="N34" s="25"/>
       <c r="O34" s="24"/>
     </row>
-    <row r="35" s="4" customFormat="1" ht="27.6" spans="1:15">
+    <row r="35" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A35" s="21" t="s">
         <v>822</v>
       </c>
@@ -56901,7 +56962,7 @@
         <v>465</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="F36" s="30" t="s">
         <v>794</v>
@@ -57066,7 +57127,7 @@
       <c r="N42" s="25"/>
       <c r="O42" s="24"/>
     </row>
-    <row r="43" customFormat="1" ht="259.2" spans="1:15">
+    <row r="43" customFormat="1" ht="261" spans="1:15">
       <c r="A43" s="21"/>
       <c r="B43" s="7"/>
       <c r="C43" s="27" t="s">
@@ -57201,7 +57262,7 @@
         <v>49</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F48" s="29" t="s">
         <v>780</v>
@@ -57378,7 +57439,7 @@
         <v>49</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F55" s="29" t="s">
         <v>780</v>
@@ -57423,7 +57484,9 @@
       <c r="O56" s="24"/>
     </row>
     <row r="57" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A57" s="21"/>
+      <c r="A57" s="55" t="s">
+        <v>833</v>
+      </c>
       <c r="B57" s="22"/>
       <c r="C57" s="35" t="s">
         <v>5</v>
@@ -57582,7 +57645,7 @@
         <v>49</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F63" s="29" t="s">
         <v>780</v>
@@ -57678,7 +57741,7 @@
     </row>
     <row r="67" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A67" s="21" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B67" s="33"/>
       <c r="C67" s="27" t="s">
@@ -57691,7 +57754,7 @@
         <v>770</v>
       </c>
       <c r="F67" s="32" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
@@ -57716,7 +57779,7 @@
         <v>803</v>
       </c>
       <c r="F68" s="30" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="G68" s="28"/>
       <c r="H68" s="29"/>
@@ -57813,7 +57876,7 @@
         <v>49</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F72" s="29" t="s">
         <v>780</v>
@@ -57830,7 +57893,7 @@
     </row>
     <row r="73" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A73" s="21" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="B73" s="33"/>
       <c r="C73" s="27" t="s">
@@ -57843,7 +57906,7 @@
         <v>770</v>
       </c>
       <c r="F73" s="32" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G73" s="29"/>
       <c r="H73" s="29"/>
@@ -57868,7 +57931,7 @@
         <v>803</v>
       </c>
       <c r="F74" s="30" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="G74" s="28"/>
       <c r="H74" s="29"/>
@@ -57965,7 +58028,7 @@
         <v>49</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F78" s="29" t="s">
         <v>780</v>

</xml_diff>